<commit_message>
Manual Testing Classwork File
</commit_message>
<xml_diff>
--- a/ManualTestingClasswork.xlsx
+++ b/ManualTestingClasswork.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783598AE-0A45-4FB8-9A0E-BE56904A662A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{837EE919-72B8-480A-9FDD-CC82746FC8F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ED6E827E-A43C-4611-A432-8F3DDE7BB4BA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
   <si>
     <t>Project Name:</t>
   </si>
@@ -130,10 +130,6 @@
     <t>Valid URL test data</t>
   </si>
   <si>
-    <t>Username: admin@erp.com
-Password: P@ssword</t>
-  </si>
-  <si>
     <t>Landed on the Home Page</t>
   </si>
   <si>
@@ -167,6 +163,46 @@
   </si>
   <si>
     <t>Username: admin@erp.com
+Password: xxxxxxxx</t>
+  </si>
+  <si>
+    <t>Still remaining on the Login Page</t>
+  </si>
+  <si>
+    <t>A popup message box to show an error message "Invalid Username/Password"</t>
+  </si>
+  <si>
+    <t>Message box got displayed</t>
+  </si>
+  <si>
+    <t>Enter an invalid username and a valid password</t>
+  </si>
+  <si>
+    <t>Enter a valid username and an invalid password</t>
+  </si>
+  <si>
+    <t>Enter an invalid username and an invalid password</t>
+  </si>
+  <si>
+    <t>1. Enter invalid username
+2. Enter valid password
+3. Click on the login button</t>
+  </si>
+  <si>
+    <t>1. Enter invalid username
+2. Enter invalid password
+3. Click on the login button</t>
+  </si>
+  <si>
+    <t>Username: xxxxxx@erp.com
+Password: P@ssw0rd</t>
+  </si>
+  <si>
+    <t>Username: admin@erp.com
+Password: P@ssw0rd</t>
+  </si>
+  <si>
+    <t>Username: xxxxxx@erp.com
 Password: xxxxxxxx</t>
   </si>
 </sst>
@@ -177,8 +213,16 @@
   <numFmts count="1">
     <numFmt numFmtId="166" formatCode="dd/mmmm/yyyy\ ddd"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -227,7 +271,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -334,11 +378,107 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -349,30 +489,364 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="dd/mmmm/yyyy\ ddd"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -383,6 +857,29 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{11AFC48B-40F2-44B1-A7B8-73016AEF342F}" name="Table1" displayName="Table1" ref="A10:N14" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+  <autoFilter ref="A10:N14" xr:uid="{11AFC48B-40F2-44B1-A7B8-73016AEF342F}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{44CCD2ED-01E0-4167-8560-19BEB6A016E0}" name="Test Scenario ID" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{36838CCE-4852-4957-B15B-3CA7B56DE936}" name="Test Scenario Description" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{10092662-DCE6-458E-8A61-AA96D3602F38}" name="Test Case ID" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{03EEB678-7E86-4887-A559-640DB59EA06D}" name="Test Case Description" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{3FB3BB1B-EF2B-44A1-9E28-05CD751F67BE}" name="Test Steps" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{B535777D-F665-446F-B66B-0AC49F29D474}" name="Pre-Condition" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{4D13C02B-7061-4C2F-B997-71EAAE279664}" name="Test Data" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{9E29A878-DFBA-4DAE-9D9E-8A817CC215C5}" name="Post-Condition" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{19393E5D-33B2-47BD-95CD-6D48C4B2D939}" name="Expected Result" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{6D437F74-24EF-455F-A396-DC54D49A38A5}" name="Actual Result" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{D8D103EB-CAA2-4006-9C97-4BB963DFCEE2}" name="Status" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{BBA95587-E891-43BE-B2D3-BEBE87326D26}" name="Executed By" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{B9A4DFDA-14A8-45E3-B71D-423D5385DFC7}" name="Execution Date" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{8CA5E39F-DFED-484C-B6B5-258E5A3CDB7C}" name="Comments (If Any)" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -684,21 +1181,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77EB142D-38D2-49EE-AAA1-8800ECE49D83}">
   <dimension ref="A2:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" customWidth="1"/>
+    <col min="1" max="1" width="14.77734375" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
     <col min="3" max="3" width="12.5546875" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="12.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
     <col min="7" max="7" width="9.77734375" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="17.77734375" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10" customWidth="1"/>
+    <col min="12" max="12" width="11.77734375" customWidth="1"/>
+    <col min="13" max="13" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:14" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -750,161 +1251,232 @@
         <v>45120</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="3" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+    <row r="10" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="J10" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="K10" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="11" t="s">
+      <c r="L10" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="M10" s="11" t="s">
+      <c r="M10" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="N10" s="11" t="s">
+      <c r="N10" s="21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="2" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
+    <row r="11" spans="1:14" s="2" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="I11" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="I11" s="12" t="s">
+      <c r="J11" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="K11" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="L11" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="L11" s="12" t="s">
+      <c r="M11" s="12">
+        <v>45107</v>
+      </c>
+      <c r="N11" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="M11" s="13">
-        <v>45108</v>
-      </c>
-      <c r="N11" s="12" t="s">
+    </row>
+    <row r="12" spans="1:14" s="2" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>36</v>
       </c>
+      <c r="D12" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="M12" s="12">
+        <v>45110</v>
+      </c>
+      <c r="N12" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="12" spans="1:14" s="1" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
+    <row r="13" spans="1:14" s="1" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="12" t="s">
+      <c r="B13" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="12" t="s">
+      <c r="D13" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H13" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
+      <c r="I13" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="L13" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="M13" s="12">
+        <v>45111</v>
+      </c>
+      <c r="N13" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="13" spans="1:14" s="1" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="12" t="s">
+    <row r="14" spans="1:14" s="1" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="12" t="s">
+      <c r="B14" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-    </row>
-    <row r="14" spans="1:14" s="1" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
+      <c r="D14" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="K14" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="L14" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="M14" s="17">
+        <v>45112</v>
+      </c>
+      <c r="N14" s="18" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="15" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>